<commit_message>
20251026 commit (N3 41Days)
</commit_message>
<xml_diff>
--- a/Words(音读音 & 训练音).xlsx
+++ b/Words(音读音 & 训练音).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\苗欣奕的东西\折跃\Japanese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E62AE9-A7D8-454F-BD8F-3E40DC4B55C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F4CE1D-75D7-48CE-8C17-086EDA76D553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object(もの)" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="818">
   <si>
     <t>木</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3508,6 +3508,38 @@
   </si>
   <si>
     <t>（刺し身）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知らせ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>しらせ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>悪い知らせがありました</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>むすめ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>違い</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ちがい</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>読書</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>どくしょ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4125,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E64ECE-FB91-4C10-BE82-49C6897072BA}">
   <dimension ref="A2:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -4337,10 +4369,10 @@
         <v>667</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>712</v>
+        <v>814</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>713</v>
+        <v>815</v>
       </c>
       <c r="K10" s="34" t="s">
         <v>714</v>
@@ -4360,10 +4392,13 @@
         <v>669</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>716</v>
+        <v>713</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -4380,10 +4415,10 @@
         <v>671</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>755</v>
+        <v>715</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -4403,10 +4438,10 @@
         <v>672</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>747</v>
+        <v>755</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>748</v>
+        <v>721</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -4426,10 +4461,10 @@
         <v>730</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>756</v>
+        <v>747</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>757</v>
+        <v>748</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -4446,10 +4481,10 @@
         <v>732</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>553</v>
+        <v>757</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -4465,6 +4500,12 @@
       <c r="F16" s="34" t="s">
         <v>752</v>
       </c>
+      <c r="I16" s="34" t="s">
+        <v>758</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="34" t="s">
@@ -4489,6 +4530,15 @@
       </c>
       <c r="B18" s="34" t="s">
         <v>750</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>811</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -6277,7 +6327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAAE8E2-4F15-4F5D-AA57-AE4D391C80DB}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -6917,10 +6967,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED5BFB1-FD88-4B4E-8145-BC2EE986EE29}">
-  <dimension ref="A2:F15"/>
+  <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7093,6 +7143,19 @@
         <v>695</v>
       </c>
     </row>
+    <row r="16" spans="1:6" ht="18">
+      <c r="A16" s="34" t="s">
+        <v>520</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="18">
+      <c r="B17" s="34" t="s">
+        <v>813</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7103,8 +7166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47639CE2-68F7-4673-A298-E034A868B499}">
   <dimension ref="A2:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7351,6 +7414,12 @@
       </c>
       <c r="C15" s="34" t="s">
         <v>587</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>816</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18">

</xml_diff>